<commit_message>
updated readme with output disclaimer.
</commit_message>
<xml_diff>
--- a/time_comparisons.xlsx
+++ b/time_comparisons.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Dropbox\Reed Group Work\Blog Posts\stationary_synth_streamflow_julia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466533AD-8DB6-484F-8E75-FFC2995FE25E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{10F5584D-E877-4C6C-A498-B17EBE7F5095}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="3390" windowWidth="16200" windowHeight="9375" xr2:uid="{9662787F-84E0-47B5-876B-6B2F8B085A86}"/>
+    <workbookView xWindow="2400" yWindow="1725" windowWidth="16200" windowHeight="9375" xr2:uid="{9662787F-84E0-47B5-876B-6B2F8B085A86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -443,7 +444,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>